<commit_message>
First commit by vishu for kitemavan
</commit_message>
<xml_diff>
--- a/TestData/vishu excel_sheet.xlsx
+++ b/TestData/vishu excel_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Viswajit\OneDrive\Desktop\Selenium sllyabus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DDFA99B-3E3E-4198-8FE8-69754D8DD658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F45FA5-4FB8-4088-84F0-2FC06DC4C3B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>DPG458</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>171992</t>
+  </si>
+  <si>
+    <t>Amol</t>
   </si>
 </sst>
 </file>
@@ -385,7 +388,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>